<commit_message>
Uploaded 15-Sep-2018 17:31:02 {/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx
+++ b/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx
@@ -1061,25 +1061,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43000000" defaultRowHeight="15.000000" customHeight="1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="29.29071508" customWidth="1" outlineLevel="0"/>
     <col min="2" max="3" width="38.86214338" customWidth="1" outlineLevel="0"/>
-    <col min="4" max="4" width="15.43357168" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="20.14785658" customWidth="1" outlineLevel="0"/>
     <col min="5" max="5" width="17.43357168" customWidth="1" outlineLevel="0"/>
     <col min="6" max="6" width="18.57642828" customWidth="1" outlineLevel="0"/>
-    <col min="7" max="7" width="35.29071317" customWidth="1" outlineLevel="0"/>
-    <col min="8" max="8" width="31.29071508" customWidth="1" outlineLevel="0"/>
-    <col min="9" max="27" width="8.00499998" customWidth="1" outlineLevel="0"/>
+    <col min="7" max="7" width="18.57642828" customWidth="1" outlineLevel="0"/>
+    <col min="8" max="8" width="35.29071317" customWidth="1" outlineLevel="0"/>
+    <col min="9" max="9" width="31.29071508" customWidth="1" outlineLevel="0"/>
+    <col min="10" max="28" width="8.00499998" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.250000" customHeight="1" outlineLevel="1">
+    <row r="1" spans="1:9" ht="14.250000" customHeight="1" outlineLevel="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="37.500000" customHeight="1" outlineLevel="1">
+    <row r="2" spans="1:9" ht="37.500000" customHeight="1" outlineLevel="1">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="37.500000" customHeight="1" outlineLevel="1">
+    <row r="3" spans="1:9" ht="37.500000" customHeight="1" outlineLevel="1">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.250000" customHeight="1" outlineLevel="1">
+    <row r="4" spans="1:9" ht="14.250000" customHeight="1" outlineLevel="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1112,11 +1113,11 @@
       </c>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:8" ht="14.250000" customHeight="1">
-      <c r="H5" s="10"/>
+    <row r="5" spans="1:9" ht="14.250000" customHeight="1">
+      <c r="I5" s="10"/>
     </row>
-    <row r="6" ht="14.250000" customHeight="1"/>
-    <row r="7" spans="1:8" ht="14.250000" customHeight="1">
+    <row r="6" spans="1:9" ht="14.250000" customHeight="1"/>
+    <row r="7" spans="1:9" ht="14.250000" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
@@ -1127,25 +1128,26 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="14.250000" customHeight="1">
+    <row r="8" spans="1:9" ht="14.250000" customHeight="1">
       <c r="A8" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>10</v>
+      <c r="B8" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>14</v>
@@ -1154,26 +1156,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.250000" customHeight="1">
-      <c r="B9" s="14"/>
-      <c r="C9" s="15" t="s">
+    <row r="9" spans="1:9" ht="14.250000" customHeight="1">
+      <c r="B9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" ht="40.500000" customHeight="1">
+    <row r="10" spans="1:9" ht="40.500000" customHeight="1">
       <c r="A10" s="13"/>
-      <c r="B10" s="15"/>
+      <c r="B10" s="15" t="s">
+        <v>16</v>
+      </c>
       <c r="C10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="15" t="s">
         <v>17</v>
       </c>
+      <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="17" t="s">
@@ -1183,24 +1185,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.750000" customHeight="1">
+    <row r="11" spans="1:9" ht="15.750000" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>24</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>25</v>
@@ -1209,23 +1211,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.250000" customHeight="1">
+    <row r="12" spans="1:9" ht="14.250000" customHeight="1">
       <c r="A12" s="20"/>
-      <c r="B12" s="21">
-        <v>7</v>
-      </c>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="22" t="b">
+      <c r="C12" s="22" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="D12" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="E12" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="22" t="s">
         <v>29</v>
+      </c>
+      <c r="F12" s="21">
+        <v>7</v>
       </c>
       <c r="G12" s="23">
         <v>12</v>
@@ -1234,23 +1236,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.250000" customHeight="1">
+    <row r="13" spans="1:9" ht="14.250000" customHeight="1">
       <c r="A13" s="20"/>
-      <c r="B13" s="21">
-        <v>7</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="22" t="b">
+      <c r="C13" s="22" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="D13" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="E13" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="22" t="s">
         <v>32</v>
+      </c>
+      <c r="F13" s="21">
+        <v>7</v>
       </c>
       <c r="G13" s="23">
         <v>12</v>
@@ -1259,23 +1261,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.250000" customHeight="1">
+    <row r="14" spans="1:9" ht="14.250000" customHeight="1">
       <c r="A14" s="20"/>
-      <c r="B14" s="21">
-        <v>7</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="22" t="b">
+      <c r="C14" s="22" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="D14" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="E14" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="22" t="s">
         <v>29</v>
+      </c>
+      <c r="F14" s="21">
+        <v>7</v>
       </c>
       <c r="G14" s="23">
         <v>3</v>
@@ -2272,7 +2274,7 @@
     <row r="1000" ht="14.250000" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.00" footer="0.00"/>

</xml_diff>

<commit_message>
Uploaded 15-Sep-2018 17:31:25 {/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx
+++ b/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43000000" defaultRowHeight="15.000000" customHeight="1" outlineLevelRow="1"/>
@@ -1146,9 +1146,7 @@
       <c r="E8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="F8" s="12"/>
       <c r="G8" s="13" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Uploaded 15-Sep-2018 17:32:07 {/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx}
</commit_message>
<xml_diff>
--- a/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx
+++ b/dm-ocb/src/main/resources/com/resources/AdhocFleetCalculation.xlsx
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43000000" defaultRowHeight="15.000000" customHeight="1" outlineLevelRow="1"/>
@@ -1127,8 +1127,6 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="14.250000" customHeight="1">
       <c r="A8" s="0" t="s">
@@ -1146,11 +1144,10 @@
       <c r="E8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="G8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1161,9 +1158,8 @@
       <c r="C9" s="16"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="14"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="40.500000" customHeight="1">
       <c r="A10" s="13"/>
@@ -1175,11 +1171,10 @@
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="G10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1199,13 +1194,10 @@
       <c r="E11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>20</v>
+      <c r="F11" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1224,13 +1216,10 @@
       <c r="E12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="21">
-        <v>7</v>
-      </c>
-      <c r="G12" s="23">
+      <c r="F12" s="23">
         <v>12</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="G12" s="23" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1249,13 +1238,10 @@
       <c r="E13" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="21">
-        <v>7</v>
-      </c>
-      <c r="G13" s="23">
+      <c r="F13" s="23">
         <v>12</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="G13" s="23" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1274,13 +1260,10 @@
       <c r="E14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="21">
-        <v>7</v>
-      </c>
-      <c r="G14" s="23">
+      <c r="F14" s="23">
         <v>3</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="G14" s="23" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>